<commit_message>
Commit new dummy data generator and new csv and xlsx with real products by ShinuyJar
</commit_message>
<xml_diff>
--- a/streamlit_browser_version/shinyjar_data.xlsx
+++ b/streamlit_browser_version/shinyjar_data.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,19 +472,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>142.63</v>
+        <v>429.11</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45937</v>
+        <v>45849</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>miscellaneous</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Taxi to meeting</t>
+          <t>Influencer collab fee</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -494,49 +494,53 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>ad</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>133.02</v>
+        <v>90</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45938</v>
+        <v>45850</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>Rings</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Coffee run</t>
+          <t>Bought 9 x Gold Ring</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>stock, sale</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>25.57</v>
+        <v>188</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45940</v>
+        <v>45852</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>miscellaneous</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TikTok ad campaign</t>
+          <t>Bought Small Jewelry Jar stock</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -546,165 +550,165 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>collab, shipping, sale</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>147.68</v>
+        <v>180</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45941</v>
+        <v>45854</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Silver wire</t>
+          <t>Bought 6 x Pearl Tie</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>supplies</t>
+          <t>sale, inventory</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>23.26</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>45945</v>
+        <v>45856</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Rings</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Lunch with supplier</t>
+          <t>Bought 5 x Gold Ring</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>PayPal</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>inventory, business</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>115.84</v>
+        <v>142.95</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>45946</v>
+        <v>45857</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tools</t>
+          <t>instagram ads</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Taxi to meeting</t>
+          <t>Bought Silver Heart Earrings stock</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>misc, stock</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>83.20999999999999</v>
+        <v>150</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45947</v>
+        <v>45857</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Gemstone beads</t>
+          <t>Bought 5 x Pearl Tie</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>urgent</t>
+          <t>urgent, collab</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>95.83</v>
+        <v>43.66</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45948</v>
+        <v>45860</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>instagram ads</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>TikTok ad campaign</t>
+          <t>Bought Vintage Watch stock</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>sale, inventory</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5.25</v>
+        <v>100</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45948</v>
+        <v>45861</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>Chokers</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Gemstone beads</t>
+          <t>Bought 4 x Chokers</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -714,53 +718,53 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>supplies</t>
+          <t>shipping, ad</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>130.61</v>
+        <v>304.45</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45949</v>
+        <v>45861</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Gold/Silver</t>
+          <t>miscellaneous</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Lunch with supplier</t>
+          <t>Bought Gold Ring stock</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>PayPal</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>urgent</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>124.78</v>
+        <v>434.36</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45952</v>
+        <v>45862</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>instagram ads</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Packaging boxes</t>
+          <t>Misc office supplies</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -770,25 +774,25 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>business, monthly</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5.05</v>
+        <v>270</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45952</v>
+        <v>45862</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>TikTok ad campaign</t>
+          <t>Bought 9 x Pearl Tie</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -796,23 +800,27 @@
           <t>Cash</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>personal, business</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>85.23999999999999</v>
+        <v>68</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45953</v>
+        <v>45862</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>Necklaces</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Lunch with supplier</t>
+          <t>Bought 4 x Pearl Necklace</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -822,77 +830,81 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>marketing</t>
+          <t>stock, personal, monthly</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>8.77</v>
+        <v>185.03</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45954</v>
+        <v>45864</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>video and image creation</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Electricity bill</t>
+          <t>Bought Pink Butterfly Earrings stock</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>collab</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>67.01000000000001</v>
+        <v>448.5</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45954</v>
+        <v>45864</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>marketing</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Studio rent</t>
+          <t>Bought Chokers stock</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr"/>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>stock, personal, business</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>121.16</v>
+        <v>18.84</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45954</v>
+        <v>45865</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>influencer ads</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Silver wire</t>
+          <t>Instagram ad campaign</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -900,183 +912,195 @@
           <t>Bank Transfer</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>collab, sale, personal</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>226.46</v>
+        <v>250</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45954</v>
+        <v>45866</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Gemstones</t>
+          <t>Chokers</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Gold chain purchase</t>
+          <t>Bought 10 x Chokers</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Card</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>monthly, inventory, sale</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>119.66</v>
+        <v>250</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45958</v>
+        <v>45867</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Chokers</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Gemstone beads</t>
+          <t>Bought 10 x Chokers</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>PayPal</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>sale, inventory</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>59.52</v>
+        <v>126.26</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45959</v>
+        <v>45868</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>miscellaneous</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Studio rent</t>
+          <t>Bought Small Jewelry Jar stock</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>personal, urgent</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>67.88</v>
+        <v>102</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45960</v>
+        <v>45868</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Gold/Silver</t>
+          <t>Earrings</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Taxi to meeting</t>
+          <t>Bought 6 x Pink Butterfly Earrings</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Cash</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>52.89</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45962</v>
+        <v>45868</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Chokers</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>TikTok ad campaign</t>
+          <t>Bought 1 x Chokers</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>PayPal</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>marketing</t>
+          <t>inventory, misc, collab</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>70.53</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45966</v>
+        <v>45868</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Electricity bill</t>
+          <t>Bought 2 x Pearl Tie</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>PayPal</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>urgent</t>
+          <t>monthly, stock, urgent</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>128.5</v>
+        <v>287.85</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45966</v>
+        <v>45870</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>video and image creation</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Silver wire</t>
+          <t>Video editing software</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1086,25 +1110,25 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>shipping</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>658.03</v>
+        <v>91</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>45966</v>
+        <v>45875</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Gold/Silver</t>
+          <t>Earrings</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Silver wire</t>
+          <t>Bought 7 x Gold Hoop Earrings</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1114,53 +1138,53 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>urgent</t>
+          <t>collab, ad, urgent</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>251.07</v>
+        <v>57.98</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>45967</v>
+        <v>45876</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Gold/Silver</t>
+          <t>transport</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Gold chain purchase</t>
+          <t>Shipping to customer</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>supplies</t>
+          <t>misc</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>131.07</v>
+        <v>60</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>45968</v>
+        <v>45876</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Electricity bill</t>
+          <t>Bought 2 x Pearl Tie</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1168,23 +1192,27 @@
           <t>Card</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>personal</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>87.66</v>
+        <v>120</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>45968</v>
+        <v>45877</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tools</t>
+          <t>Earrings</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Studio rent</t>
+          <t>Bought 10 x Silver Heart Earrings</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1194,133 +1222,137 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>sale, misc</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>44.84</v>
+        <v>435.03</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>45969</v>
+        <v>45877</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>miscellaneous</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Lunch with supplier</t>
+          <t>Bought Pearl Tie stock</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Cash</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>urgent, ad, personal</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>800</v>
+        <v>84</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45971</v>
+        <v>45878</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Instagram Ads</t>
+          <t>Rings</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Gemstone beads</t>
+          <t>Bought 7 x Silver Turtle Ring</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>marketing</t>
+          <t>stock, shipping</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>48.67</v>
+        <v>60</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45972</v>
+        <v>45879</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Rings</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Coffee run</t>
+          <t>Bought 5 x Silver Turtle Ring</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>personal, misc, stock</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>256.53</v>
+        <v>150</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45973</v>
+        <v>45880</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Instagram Ads</t>
+          <t>Watches</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Studio rent</t>
+          <t>Bought 3 x Vintage Watch</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>inventory, shipping</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>65.15000000000001</v>
+        <v>136</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45974</v>
+        <v>45881</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Necklaces</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Coffee run</t>
+          <t>Bought 8 x Pearl Necklace</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1330,25 +1362,25 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>supplies</t>
+          <t>inventory</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>137.25</v>
+        <v>25</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45975</v>
+        <v>45882</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Watches</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Electricity bill</t>
+          <t>Bought 1 x Children's Watch</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1358,25 +1390,25 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>collab</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>137.01</v>
+        <v>50</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45976</v>
+        <v>45886</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Gemstones</t>
+          <t>Earrings</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Packaging boxes</t>
+          <t>Bought 5 x Small Earrings</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1386,53 +1418,53 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>marketing</t>
+          <t>personal, stock, inventory</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>149.6</v>
+        <v>36</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>45977</v>
+        <v>45887</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Rings</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Packaging boxes</t>
+          <t>Bought 3 x Silver Turtle Ring</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
+          <t>Card</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>urgent</t>
+          <t>urgent, collab, personal</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>377.51</v>
+        <v>409.05</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45977</v>
+        <v>45888</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Gold/Silver</t>
+          <t>video and image creation</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Instagram boosted post</t>
+          <t>Bought Silver Heart Earrings stock</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1442,77 +1474,81 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>collab, inventory, sale</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>105.07</v>
+        <v>150</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45981</v>
+        <v>45891</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>Bracelets</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Lunch with supplier</t>
+          <t>Bought 10 x Gold Bracelet</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
+          <t>PayPal</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>business, misc</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>11.93</v>
+        <v>119</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45984</v>
+        <v>45893</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Tools</t>
+          <t>Necklaces</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Coffee run</t>
+          <t>Bought 7 x Pearl Necklace</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>PayPal</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>inventory, sale</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>606.53</v>
+        <v>203.64</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45985</v>
+        <v>45896</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Gold/Silver</t>
+          <t>influencer ads</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Silver wire</t>
+          <t>Bought Silver Bracelet stock</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1520,23 +1556,27 @@
           <t>Cash</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr"/>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>monthly, urgent</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>118.01</v>
+        <v>27.95</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>45987</v>
+        <v>45896</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>instagram ads</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Electricity bill</t>
+          <t>Bought Pearl Necklace stock</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1546,25 +1586,25 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>supplies</t>
+          <t>monthly</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>36.19</v>
+        <v>338.44</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45987</v>
+        <v>45900</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>miscellaneous</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Instagram boosted post</t>
+          <t>Bought Silver Bracelet stock</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1574,157 +1614,165 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>sale</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>11.56</v>
+        <v>105</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>45989</v>
+        <v>45901</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Bracelets</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Packaging boxes</t>
+          <t>Bought 7 x Gold Bracelet</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>PayPal</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr"/>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>misc, collab</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>94.45999999999999</v>
+        <v>133.94</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>45989</v>
+        <v>45901</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Gemstones</t>
+          <t>influencer ads</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Gold chain purchase</t>
+          <t>Bought Gold Ring stock</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>PayPal</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>personal, inventory, misc</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>23.67</v>
+        <v>280</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>45990</v>
+        <v>45903</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Jewelry Supplies</t>
+          <t>Jars</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Silver wire</t>
+          <t>Bought 7 x Shiny Jewelry Jar</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>collab, stock, shipping</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>70.70999999999999</v>
+        <v>45</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>45990</v>
+        <v>45907</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Bracelets</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Packaging boxes</t>
+          <t>Bought 3 x Silver Bracelet</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr"/>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>collab</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>329.45</v>
+        <v>170</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>45991</v>
+        <v>45908</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Instagram Ads</t>
+          <t>Earrings</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Gemstone beads</t>
+          <t>Bought 10 x Pink Butterfly Earrings</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>ad</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>103.87</v>
+        <v>300</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>45991</v>
+        <v>45908</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Jewelry Supplies</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Lunch with supplier</t>
+          <t>Bought 10 x Pearl Tie</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1740,80 +1788,80 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>117.96</v>
+        <v>303.42</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>45992</v>
+        <v>45909</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>transport</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Studio rent</t>
+          <t>Bought Silver Bracelet stock</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Card</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>urgent</t>
+          <t>stock</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>73.38</v>
+        <v>60</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>45993</v>
+        <v>45910</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Tools</t>
+          <t>Rings</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Gemstone beads</t>
+          <t>Bought 5 x Silver Turtle Ring</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
+          <t>Card</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>marketing</t>
+          <t>urgent, ad, personal</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>236.58</v>
+        <v>200</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>45995</v>
+        <v>45911</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Instagram Ads</t>
+          <t>Jars</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>New pliers set</t>
+          <t>Bought 5 x Shiny Jewelry Jar</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -1824,131 +1872,131 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>41.57</v>
+        <v>85</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>45996</v>
+        <v>45911</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Jewelry Supplies</t>
+          <t>Necklaces</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Silver wire</t>
+          <t>Bought 5 x Pearl Necklace</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>monthly, misc</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>39.51</v>
+        <v>341.55</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>45997</v>
+        <v>45912</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>influencer ads</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Gemstone beads</t>
+          <t>Taxi to supplier</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>Card</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>business, inventory, sale</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>68.79000000000001</v>
+        <v>243.75</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>45998</v>
+        <v>45914</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>instagram ads</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Lunch with supplier</t>
+          <t>Bought Small Jewelry Jar stock</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>ad</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>649.34</v>
+        <v>47.12</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>45998</v>
+        <v>45915</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Instagram Ads</t>
+          <t>marketing</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Packaging boxes</t>
+          <t>Image creation tools</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>inventory</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>123.06</v>
+        <v>82.11</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>45999</v>
+        <v>45916</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>instagram ads</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Taxi to meeting</t>
+          <t>Bought Gold Ring stock</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1958,25 +2006,25 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>marketing</t>
+          <t>monthly, urgent, collab</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>33.97</v>
+        <v>13.42</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>46000</v>
+        <v>45916</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>instagram ads</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Electricity bill</t>
+          <t>Influencer collab fee</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1986,53 +2034,53 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>marketing</t>
+          <t>sale, collab, shipping</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>63.95</v>
+        <v>156.19</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>46006</v>
+        <v>45917</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Jewelry Supplies</t>
+          <t>influencer ads</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>New pliers set</t>
+          <t>Influencer collab fee</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Card</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>supplies</t>
+          <t>inventory, misc</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>136.52</v>
+        <v>291.29</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>46007</v>
+        <v>45917</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>influencer ads</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Instagram boosted post</t>
+          <t>Bought Pearl Necklace stock</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2042,325 +2090,333 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>marketing</t>
+          <t>sale, inventory</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>64.77</v>
+        <v>75.75</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>46008</v>
+        <v>45922</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>influencer ads</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Gold chain purchase</t>
+          <t>Bought Pearl Tie stock</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>shipping, stock</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>70.87</v>
+        <v>200</v>
       </c>
       <c r="B61" s="2" t="n">
-        <v>46008</v>
+        <v>45923</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Jars</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>New pliers set</t>
+          <t>Bought 10 x Small Jewelry Jar</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Card</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr"/>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>urgent</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>131.63</v>
+        <v>30</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>46008</v>
+        <v>45924</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Rings</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Studio rent</t>
+          <t>Bought 3 x Gold Ring</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>marketing</t>
+          <t>business, ad, personal</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>82.79000000000001</v>
+        <v>50</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>46009</v>
+        <v>45926</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Watches</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Silver wire</t>
+          <t>Bought 1 x Vintage Watch</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>PayPal</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>supplies</t>
+          <t>stock</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>87.31999999999999</v>
+        <v>170</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>46009</v>
+        <v>45927</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Necklaces</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>TikTok ad campaign</t>
+          <t>Bought 10 x Pearl Necklace</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>misc, monthly, stock</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>609.41</v>
+        <v>60</v>
       </c>
       <c r="B65" s="2" t="n">
-        <v>46010</v>
+        <v>45927</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Gemstones</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Coffee run</t>
+          <t>Bought 2 x Pearl Tie</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>PayPal</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr"/>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>misc, collab, sale</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>776.95</v>
+        <v>17</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>46011</v>
+        <v>45930</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Gemstones</t>
+          <t>Necklaces</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Lunch with supplier</t>
+          <t>Bought 1 x Pearl Necklace</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>urgent</t>
+          <t>personal, misc</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>81.33</v>
+        <v>112.94</v>
       </c>
       <c r="B67" s="2" t="n">
-        <v>46012</v>
+        <v>45930</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>influencer ads</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Taxi to meeting</t>
+          <t>Bought Shiny Jewelry Jar stock</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>business, ad</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>17.66</v>
+        <v>330.54</v>
       </c>
       <c r="B68" s="2" t="n">
-        <v>46014</v>
+        <v>45932</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>video and image creation</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>New pliers set</t>
+          <t>Bought Children's Watch stock</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>personal, shipping</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>602.66</v>
+        <v>180</v>
       </c>
       <c r="B69" s="2" t="n">
-        <v>46015</v>
+        <v>45936</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Gemstones</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Instagram boosted post</t>
+          <t>Bought 6 x Pearl Tie</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>Card</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>urgent</t>
+          <t>collab</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>64.67</v>
+        <v>350</v>
       </c>
       <c r="B70" s="2" t="n">
-        <v>46015</v>
+        <v>45939</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Watches</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Packaging boxes</t>
+          <t>Bought 7 x Vintage Watch</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Card</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>urgent</t>
+          <t>business, collab, shipping</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>104.78</v>
+        <v>449.76</v>
       </c>
       <c r="B71" s="2" t="n">
-        <v>46018</v>
+        <v>45940</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Tools</t>
+          <t>video and image creation</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Silver wire</t>
+          <t>Bought Shiny Jewelry Jar stock</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2368,23 +2424,27 @@
           <t>Card</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr"/>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>inventory</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>591.34</v>
+        <v>154.55</v>
       </c>
       <c r="B72" s="2" t="n">
-        <v>46019</v>
+        <v>45940</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Gold/Silver</t>
+          <t>video and image creation</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Taxi to meeting</t>
+          <t>Bought Silver Heart Earrings stock</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2394,165 +2454,165 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>urgent</t>
+          <t>personal, inventory</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>27.49</v>
+        <v>105</v>
       </c>
       <c r="B73" s="2" t="n">
-        <v>46020</v>
+        <v>45941</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Packaging</t>
+          <t>Bracelets</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>TikTok ad campaign</t>
+          <t>Bought 7 x Silver Bracelet</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Card</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>supplies</t>
+          <t>monthly</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>119.17</v>
+        <v>60</v>
       </c>
       <c r="B74" s="2" t="n">
-        <v>46020</v>
+        <v>45941</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Gold/Silver</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Taxi to meeting</t>
+          <t>Bought 2 x Pearl Tie</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>shipping</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>68.05</v>
+        <v>223.81</v>
       </c>
       <c r="B75" s="2" t="n">
-        <v>46020</v>
+        <v>45943</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Gemstones</t>
+          <t>instagram ads</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>TikTok ad campaign</t>
+          <t>Bought Silver Bracelet stock</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>PayPal</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>personal</t>
+          <t>shipping</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>140.95</v>
+        <v>45</v>
       </c>
       <c r="B76" s="2" t="n">
-        <v>46022</v>
+        <v>45943</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Instagram Ads</t>
+          <t>Bracelets</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Gold chain purchase</t>
+          <t>Bought 3 x Silver Bracelet</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>Bank Transfer</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>monthly</t>
+          <t>misc, sale</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>29.44</v>
+        <v>136</v>
       </c>
       <c r="B77" s="2" t="n">
-        <v>46022</v>
+        <v>45944</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Necklaces</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Coffee run</t>
+          <t>Bought 8 x Pearl Necklace</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>Cash</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>urgent</t>
+          <t>misc, sale, shipping</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>217.67</v>
+        <v>85</v>
       </c>
       <c r="B78" s="2" t="n">
-        <v>46023</v>
+        <v>45944</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Gold/Silver</t>
+          <t>Necklaces</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>TikTok ad campaign</t>
+          <t>Bought 5 x Pearl Necklace</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2560,87 +2620,2055 @@
           <t>Cash</t>
         </is>
       </c>
-      <c r="F78" t="inlineStr"/>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>inventory, shipping, monthly</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>50.77</v>
+        <v>210</v>
       </c>
       <c r="B79" s="2" t="n">
-        <v>46023</v>
+        <v>45945</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Electricity bill</t>
+          <t>Bought 7 x Pearl Tie</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Cash</t>
+          <t>PayPal</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>marketing</t>
+          <t>business, urgent</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>89.79000000000001</v>
+        <v>412.6</v>
       </c>
       <c r="B80" s="2" t="n">
-        <v>46024</v>
+        <v>45946</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Tools</t>
+          <t>marketing</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Lunch with supplier</t>
+          <t>Bought Small Jewelry Jar stock</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Card</t>
+          <t>PayPal</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>supplies</t>
+          <t>monthly</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>106.22</v>
+        <v>60</v>
       </c>
       <c r="B81" s="2" t="n">
-        <v>46025</v>
+        <v>45948</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Tools</t>
+          <t>Ties</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Gemstone beads</t>
+          <t>Bought 2 x Pearl Tie</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>monthly, personal, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>60</v>
+      </c>
+      <c r="B82" s="2" t="n">
+        <v>45948</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Bracelets</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Bought 4 x Silver Bracelet</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>business, shipping, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>300</v>
+      </c>
+      <c r="B83" s="2" t="n">
+        <v>45949</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Jars</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Bought 3 x Big Jewelry Jar</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
           <t>PayPal</t>
         </is>
       </c>
-      <c r="F81" t="inlineStr"/>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>321</v>
+      </c>
+      <c r="B84" s="2" t="n">
+        <v>45950</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Marketing flyers</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>business, collab</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>17</v>
+      </c>
+      <c r="B85" s="2" t="n">
+        <v>45952</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Necklaces</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Bought 1 x Pearl Necklace</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>personal, collab</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>308.36</v>
+      </c>
+      <c r="B86" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Bought Silver Bracelet stock</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>257.08</v>
+      </c>
+      <c r="B87" s="2" t="n">
+        <v>45958</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>miscellaneous</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Bought Small Jewelry Jar stock</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>collab</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>120</v>
+      </c>
+      <c r="B88" s="2" t="n">
+        <v>45959</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Bracelets</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Bought 8 x Gold Bracelet</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>160</v>
+      </c>
+      <c r="B89" s="2" t="n">
+        <v>45960</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Jars</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Bought 8 x Small Jewelry Jar</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>business, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>33.73</v>
+      </c>
+      <c r="B90" s="2" t="n">
+        <v>45961</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Bought Silver Turtle Ring stock</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>collab, personal, ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>348.73</v>
+      </c>
+      <c r="B91" s="2" t="n">
+        <v>45962</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Bought Gold Bracelet stock</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>250</v>
+      </c>
+      <c r="B92" s="2" t="n">
+        <v>45962</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Watches</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Bought 5 x Vintage Watch</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>business, sale, collab</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>60</v>
+      </c>
+      <c r="B93" s="2" t="n">
+        <v>45962</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Bought 5 x Silver Heart Earrings</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>175</v>
+      </c>
+      <c r="B94" s="2" t="n">
+        <v>45962</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Chokers</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Bought 7 x Chokers</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>urgent, shipping</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>185.04</v>
+      </c>
+      <c r="B95" s="2" t="n">
+        <v>45962</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Bought Small Jewelry Jar stock</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>shipping, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>368.24</v>
+      </c>
+      <c r="B96" s="2" t="n">
+        <v>45963</v>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>miscellaneous</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Marketing flyers</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>misc, business, personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>60</v>
+      </c>
+      <c r="B97" s="2" t="n">
+        <v>45964</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Bracelets</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Bought 4 x Gold Bracelet</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>253.35</v>
+      </c>
+      <c r="B98" s="2" t="n">
+        <v>45964</v>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Bought Children's Watch stock</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>75</v>
+      </c>
+      <c r="B99" s="2" t="n">
+        <v>45966</v>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Chokers</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Bought 3 x Chokers</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>inventory, urgent, sale</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>136</v>
+      </c>
+      <c r="B100" s="2" t="n">
+        <v>45967</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Bought 8 x Pink Butterfly Earrings</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>misc, sale</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>150</v>
+      </c>
+      <c r="B101" s="2" t="n">
+        <v>45971</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Bracelets</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Bought 10 x Silver Bracelet</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>ad, inventory</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>300</v>
+      </c>
+      <c r="B102" s="2" t="n">
+        <v>45972</v>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Watches</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Bought 6 x Vintage Watch</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>stock, collab, personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>422.03</v>
+      </c>
+      <c r="B103" s="2" t="n">
+        <v>45973</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Image creation tools</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>collab, stock, sale</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>100</v>
+      </c>
+      <c r="B104" s="2" t="n">
+        <v>45973</v>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Bought 10 x Small Earrings</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>monthly, shipping, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>12</v>
+      </c>
+      <c r="B105" s="2" t="n">
+        <v>45976</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Rings</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Bought 1 x Silver Turtle Ring</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>ad, stock, inventory</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>12</v>
+      </c>
+      <c r="B106" s="2" t="n">
+        <v>45976</v>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Rings</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Bought 1 x Silver Turtle Ring</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>72</v>
+      </c>
+      <c r="B107" s="2" t="n">
+        <v>45976</v>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Bought 6 x Silver Heart Earrings</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>collab, misc</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>300</v>
+      </c>
+      <c r="B108" s="2" t="n">
+        <v>45978</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Ties</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Bought 10 x Pearl Tie</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>55.19</v>
+      </c>
+      <c r="B109" s="2" t="n">
+        <v>45978</v>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>miscellaneous</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Video editing software</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>68</v>
+      </c>
+      <c r="B110" s="2" t="n">
+        <v>45978</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Bought 4 x Pink Butterfly Earrings</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="B111" s="2" t="n">
+        <v>45981</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>instagram ads</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Video editing software</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>sale, ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>105</v>
+      </c>
+      <c r="B112" s="2" t="n">
+        <v>45986</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Bracelets</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Bought 7 x Gold Bracelet</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>stock, business, sale</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>300</v>
+      </c>
+      <c r="B113" s="2" t="n">
+        <v>45986</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Watches</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Bought 6 x Vintage Watch</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>shipping, misc</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>30</v>
+      </c>
+      <c r="B114" s="2" t="n">
+        <v>45986</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Bought 3 x Small Earrings</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>shipping, misc</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>45</v>
+      </c>
+      <c r="B115" s="2" t="n">
+        <v>45989</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Bracelets</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Bought 3 x Gold Bracelet</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>inventory, misc</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>102</v>
+      </c>
+      <c r="B116" s="2" t="n">
+        <v>45989</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Necklaces</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Bought 6 x Pearl Necklace</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>120</v>
+      </c>
+      <c r="B117" s="2" t="n">
+        <v>45989</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Bought 10 x Silver Heart Earrings</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>misc</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>200</v>
+      </c>
+      <c r="B118" s="2" t="n">
+        <v>45990</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Jars</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Bought 10 x Small Jewelry Jar</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>ad, shipping</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>70</v>
+      </c>
+      <c r="B119" s="2" t="n">
+        <v>45990</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Rings</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Bought 7 x Gold Ring</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>shipping</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>150</v>
+      </c>
+      <c r="B120" s="2" t="n">
+        <v>45993</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Watches</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Bought 3 x Vintage Watch</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>misc, personal, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>308.3</v>
+      </c>
+      <c r="B121" s="2" t="n">
+        <v>45994</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>influencer ads</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Bought Gold Bracelet stock</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>inventory, monthly, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>152.64</v>
+      </c>
+      <c r="B122" s="2" t="n">
+        <v>45996</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>video and image creation</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Bought Gold Ring stock</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>business</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>60</v>
+      </c>
+      <c r="B123" s="2" t="n">
+        <v>45998</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Bought 6 x Small Earrings</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>stock, personal, monthly</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>120</v>
+      </c>
+      <c r="B124" s="2" t="n">
+        <v>45999</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Bracelets</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Bought 8 x Silver Bracelet</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>inventory</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>366.31</v>
+      </c>
+      <c r="B125" s="2" t="n">
+        <v>45999</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>video and image creation</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Bought Vintage Watch stock</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>business, stock, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>39</v>
+      </c>
+      <c r="B126" s="2" t="n">
+        <v>46002</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Bought 3 x Gold Hoop Earrings</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>urgent, misc, business</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>100</v>
+      </c>
+      <c r="B127" s="2" t="n">
+        <v>46003</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Chokers</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Bought 4 x Chokers</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>stock, shipping, inventory</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>91.34</v>
+      </c>
+      <c r="B128" s="2" t="n">
+        <v>46004</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Bought Shiny Jewelry Jar stock</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>ad, stock</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>125</v>
+      </c>
+      <c r="B129" s="2" t="n">
+        <v>46005</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Watches</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Bought 5 x Children's Watch</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>120</v>
+      </c>
+      <c r="B130" s="2" t="n">
+        <v>46006</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Jars</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Bought 3 x Shiny Jewelry Jar</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>60</v>
+      </c>
+      <c r="B131" s="2" t="n">
+        <v>46007</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Bought 5 x Silver Heart Earrings</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>misc, stock, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>485.67</v>
+      </c>
+      <c r="B132" s="2" t="n">
+        <v>46007</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Bought Silver Heart Earrings stock</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>sale, shipping, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>166.66</v>
+      </c>
+      <c r="B133" s="2" t="n">
+        <v>46008</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>influencer ads</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Bought Chokers stock</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>inventory</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>80</v>
+      </c>
+      <c r="B134" s="2" t="n">
+        <v>46010</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Rings</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Bought 8 x Gold Ring</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>misc, shipping, urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>130.13</v>
+      </c>
+      <c r="B135" s="2" t="n">
+        <v>46012</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>influencer ads</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Bought Gold Ring stock</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>urgent, collab</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>104</v>
+      </c>
+      <c r="B136" s="2" t="n">
+        <v>46012</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Bought 8 x Gold Hoop Earrings</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>PayPal</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>business, collab</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>40</v>
+      </c>
+      <c r="B137" s="2" t="n">
+        <v>46014</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Jars</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Bought 1 x Shiny Jewelry Jar</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>misc</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>91.3</v>
+      </c>
+      <c r="B138" s="2" t="n">
+        <v>46015</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>video and image creation</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Bought Small Jewelry Jar stock</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>sale, collab, ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>30</v>
+      </c>
+      <c r="B139" s="2" t="n">
+        <v>46016</v>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Bracelets</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Bought 2 x Silver Bracelet</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>59.33</v>
+      </c>
+      <c r="B140" s="2" t="n">
+        <v>46016</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Bought Silver Heart Earrings stock</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>85</v>
+      </c>
+      <c r="B141" s="2" t="n">
+        <v>46019</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Necklaces</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Bought 5 x Pearl Necklace</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>business</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>60</v>
+      </c>
+      <c r="B142" s="2" t="n">
+        <v>46019</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Ties</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Bought 2 x Pearl Tie</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>misc</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>350</v>
+      </c>
+      <c r="B143" s="2" t="n">
+        <v>46020</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Watches</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Bought 7 x Vintage Watch</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>inventory, personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>80</v>
+      </c>
+      <c r="B144" s="2" t="n">
+        <v>46021</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Earrings</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Bought 8 x Small Earrings</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>urgent</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>190.77</v>
+      </c>
+      <c r="B145" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>video and image creation</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Bought Chokers stock</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>stock, personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>428.53</v>
+      </c>
+      <c r="B146" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>video and image creation</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Bought Small Earrings stock</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>business, ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>75</v>
+      </c>
+      <c r="B147" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Bracelets</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Bought 5 x Gold Bracelet</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>misc, business</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>460.54</v>
+      </c>
+      <c r="B148" s="2" t="n">
+        <v>46027</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>miscellaneous</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Bought Silver Turtle Ring stock</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>personal</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>175.79</v>
+      </c>
+      <c r="B149" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Bought Pink Butterfly Earrings stock</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>210</v>
+      </c>
+      <c r="B150" s="2" t="n">
+        <v>46028</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Ties</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Bought 7 x Pearl Tie</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>180</v>
+      </c>
+      <c r="B151" s="2" t="n">
+        <v>46029</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Ties</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Bought 6 x Pearl Tie</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>urgent, sale</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2653,7 +4681,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2691,11 +4719,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jewelry Supplies</t>
+          <t>Jars</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1200</v>
+        <v>950.64</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -2710,11 +4738,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Watches</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>400</v>
+        <v>720.6</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2729,11 +4757,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Instagram Ads</t>
+          <t>Bracelets</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1250</v>
+        <v>1076.51</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -2748,11 +4776,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Necklaces</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>250</v>
+        <v>840.9400000000001</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -2767,11 +4795,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>Rings</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>300</v>
+        <v>1335.05</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -2786,11 +4814,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>overall</t>
+          <t>Earrings</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6000</v>
+        <v>529.78</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -2801,6 +4829,177 @@
         <v>45992</v>
       </c>
       <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ties</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>574.65</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Chokers</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1132.55</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>771.6799999999999</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>marketing</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>562.16</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>instagram ads</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>543.37</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>video and image creation</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1250.46</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>influencer ads</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>229.055</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>miscellaneous</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1193.73</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>monthly</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>